<commit_message>
Project 1 finished, homework 4 finished
</commit_message>
<xml_diff>
--- a/Homework04/Data Tables_HW4.xlsx
+++ b/Homework04/Data Tables_HW4.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Simulated DC" sheetId="2" r:id="rId2"/>
     <sheet name="AC" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -271,13 +271,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,6 +306,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -315,7 +321,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -338,15 +344,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -373,6 +406,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,7 +691,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -657,7 +702,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,359 +713,359 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>4</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>2</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>4</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>2</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <f>C6</f>
         <v>469.53949999999998</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <f>F6</f>
         <v>469.53949999999998</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <f>E6</f>
         <v>939.07899999999995</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <f>2*F6</f>
         <v>939.07899999999995</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>469.53949999999998</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>1.3187</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <f>F7</f>
         <v>2.3098999999999998</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>1.6334</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <f>F7</f>
         <v>2.3098999999999998</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>2.3098999999999998</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="2"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <f>B11-B13</f>
         <v>1.8916999999999999</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <f t="shared" ref="C9:F9" si="0">C11-C13</f>
         <v>-2.9569000000000001</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <f t="shared" si="0"/>
         <v>-2.2804000000000002</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <f t="shared" si="0"/>
         <v>-2.9569000000000001</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>-2.9569000000000001</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <f>B12-B13</f>
         <v>2.7195999999999998</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <f t="shared" ref="C10:F10" si="1">C12-C13</f>
         <v>-7.2804000000000002</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <f t="shared" si="1"/>
         <v>-5</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <f t="shared" si="1"/>
         <v>-5</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <f t="shared" si="1"/>
         <v>-2.9569000000000001</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>1.8916999999999999</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <f>F11</f>
         <v>7.0430999999999999</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>2.7195999999999998</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <f>F11</f>
         <v>7.0430999999999999</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>7.0430999999999999</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <f>D11</f>
         <v>2.7195999999999998</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <f>D11</f>
         <v>2.7195999999999998</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>0</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>5</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <f>F11</f>
         <v>7.0430999999999999</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>0</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>10</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>5</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>10</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>10</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="2"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>712.1114</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>406.54379999999998</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>1149.9000000000001</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>813.08770000000004</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>406.54379999999998</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <f>1/B17*1000</f>
         <v>7.7474036513513411</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <f t="shared" ref="C16:F16" si="2">1/C17*1000</f>
         <v>10.282913807588173</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <f t="shared" si="2"/>
         <v>20.565848762861368</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <f t="shared" si="2"/>
         <v>20.565848762861368</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <f t="shared" si="2"/>
         <v>10.282913807588173</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>129.07550000000001</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>97.248699999999999</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>48.624299999999998</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>48.624299999999998</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>97.248699999999999</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1049,355 +1094,355 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>4</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>2</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>4</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>2</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <f>C6</f>
         <v>515.9</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>515.9</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <f>E6</f>
         <v>988.2</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>988.2</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>473.6</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>1.3520000000000001</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>2.25</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>1.591</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>2.25</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>2.25</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="2"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <f t="shared" ref="B9:E9" si="0">B11-B13</f>
         <v>1.925</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <f t="shared" si="0"/>
         <v>-2.8970000000000002</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <f t="shared" si="0"/>
         <v>-2.238</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <f t="shared" si="0"/>
         <v>-2.8970000000000002</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <f>F11-F13</f>
         <v>-2.8970000000000002</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <f t="shared" ref="B10:E10" si="1">B12-B13</f>
         <v>2.762</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <f t="shared" si="1"/>
         <v>-7.2379999999999995</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <f t="shared" si="1"/>
         <v>-5</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <f t="shared" si="1"/>
         <v>-5</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <f>F12-F13</f>
         <v>-2.8970000000000002</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>1.925</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <f>F11</f>
         <v>7.1029999999999998</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>2.762</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <f>F11</f>
         <v>7.1029999999999998</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>7.1029999999999998</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <f>D11</f>
         <v>2.762</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <f>D11</f>
         <v>2.762</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>0</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>5</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <f>F11</f>
         <v>7.1029999999999998</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>0</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>10</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>5</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>10</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>10</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="2"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>763.3</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>458.7</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>1242</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>878.5</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>421</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>8.141</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>9.7530000000000001</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>19.5</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>19.510000000000002</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <v>9.7530000000000001</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <f t="shared" ref="B17:D17" si="2">1/B16*1000</f>
         <v>122.83503255128363</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <f t="shared" si="2"/>
         <v>102.53255408592229</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <f t="shared" si="2"/>
         <v>51.282051282051277</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <f>1/E16*1000</f>
         <v>51.255766273705788</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <f>1/F16*1000</f>
         <v>102.53255408592229</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1411,127 +1456,165 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="10"/>
-    <col min="2" max="2" width="10.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="12" style="9" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="2">
+      <c r="B2" s="4">
+        <v>839.62260000000003</v>
+      </c>
+      <c r="C2" s="1">
         <v>796.4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
+      <c r="B4" s="1">
+        <v>31.6249</v>
+      </c>
+      <c r="C4" s="1">
+        <f>20*LOG10(ABS(G4))</f>
+        <v>32.329510277771313</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="G4" s="11">
+        <v>41.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
+      <c r="B6" s="1">
+        <v>31.553000000000001</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ref="C5:C10" si="0">20*LOG10(ABS(G6))</f>
+        <v>32.264147042075194</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="G6" s="13">
+        <v>41.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
+      <c r="B8" s="1">
+        <v>30.9253</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>31.677571969972519</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="G8" s="13">
+        <v>38.36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
+      <c r="B10" s="1">
+        <v>26.331</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>27.320984196004709</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="G10" s="13">
+        <v>23.23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>